<commit_message>
[LC-943] Update documentation for Letsco OS 1.3.1
Signed-off-by: OUESLATI Wyem Ext <wyem.oueslati@rte-france.com>
</commit_message>
<xml_diff>
--- a/_site/documentation/asciidoc/user_manual/attached_doc/serviceA_allKpis_7RSCs_2021_2025.xlsx
+++ b/_site/documentation/asciidoc/user_manual/attached_doc/serviceA_allKpis_7RSCs_2021_2025.xlsx
@@ -6,15 +6,15 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="GP1" r:id="rId3" sheetId="1"/>
-    <sheet name="GP2" r:id="rId4" sheetId="2"/>
-    <sheet name="BP1" r:id="rId5" sheetId="3"/>
-    <sheet name="BP2" r:id="rId6" sheetId="4"/>
-    <sheet name="BP3" r:id="rId7" sheetId="5"/>
-    <sheet name="BP4" r:id="rId8" sheetId="6"/>
-    <sheet name="BP5" r:id="rId9" sheetId="7"/>
-    <sheet name="BP6" r:id="rId10" sheetId="8"/>
-    <sheet name="BP7" r:id="rId11" sheetId="9"/>
+    <sheet name="GP01" r:id="rId3" sheetId="1"/>
+    <sheet name="GP02" r:id="rId4" sheetId="2"/>
+    <sheet name="BP01" r:id="rId5" sheetId="3"/>
+    <sheet name="BP02" r:id="rId6" sheetId="4"/>
+    <sheet name="BP03" r:id="rId7" sheetId="5"/>
+    <sheet name="BP04" r:id="rId8" sheetId="6"/>
+    <sheet name="BP05" r:id="rId9" sheetId="7"/>
+    <sheet name="BP06" r:id="rId10" sheetId="8"/>
+    <sheet name="BP07" r:id="rId11" sheetId="9"/>
   </sheets>
 </workbook>
 </file>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="17">
   <si>
-    <t>KPI GP1 - Global Perf 1</t>
+    <t>KPI GP01 - Global Perf 1</t>
   </si>
   <si>
     <t>Date</t>
@@ -49,28 +49,28 @@
     <t>TSCNET</t>
   </si>
   <si>
-    <t>KPI GP2 - Global Perf 2</t>
+    <t>KPI GP02 - Global Perf 2</t>
   </si>
   <si>
-    <t>KPI BP1 - Business Process 1</t>
+    <t>KPI BP01 - Business Process 1</t>
   </si>
   <si>
-    <t>KPI BP2 - Business Process 2</t>
+    <t>KPI BP02 - Business Process 2</t>
   </si>
   <si>
-    <t>KPI BP3 - Business Process 3</t>
+    <t>KPI BP03 - Business Process 3</t>
   </si>
   <si>
-    <t>KPI BP4 - Business Process 4</t>
+    <t>KPI BP04 - Business Process 4</t>
   </si>
   <si>
-    <t>KPI BP5 - Business Process 5</t>
+    <t>KPI BP05 - Business Process 5</t>
   </si>
   <si>
-    <t>KPI BP6 - Business Process 6</t>
+    <t>KPI BP06 - Business Process 6</t>
   </si>
   <si>
-    <t>KPI BP7 - Business Process 7</t>
+    <t>KPI BP07 - Business Process 7</t>
   </si>
 </sst>
 </file>

</xml_diff>